<commit_message>
started loop pt 2
</commit_message>
<xml_diff>
--- a/Experimet-1 Validation Accuracy Table.xlsx
+++ b/Experimet-1 Validation Accuracy Table.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rgurlek\Box\Okul\Deep Learning\Music-Classification\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jgomezm\OneDrive - Emory University\Course Work\Spring 2020\CS 584 - Deep Learning\Class Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45D5307B-C4FD-4756-BF55-BA9995A9D671}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{45D5307B-C4FD-4756-BF55-BA9995A9D671}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{DD33AB27-D312-486B-B38F-7EB09BFA0ABF}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="val" sheetId="1" r:id="rId1"/>
@@ -72,7 +72,7 @@
     <t>Sampling Rate</t>
   </si>
   <si>
-    <t>Samplin Window</t>
+    <t>Sampling Window</t>
   </si>
 </sst>
 </file>
@@ -396,7 +396,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -550,9 +550,7 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
+      <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -563,14 +561,71 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
+      <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -619,23 +674,43 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="43">
@@ -996,7 +1071,7 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+      <selection activeCell="D3" sqref="D1:H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1006,25 +1081,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="20"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2">
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="16">
         <v>1</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="21">
         <v>10</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="22">
         <v>100</v>
       </c>
     </row>
@@ -1035,19 +1110,19 @@
       <c r="B3">
         <v>0.13045833110809299</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="9">
+      <c r="E3" s="15">
         <v>1</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="4">
         <v>0.13045833110809299</v>
       </c>
-      <c r="G3" s="6">
+      <c r="G3" s="5">
         <v>0.153333333134651</v>
       </c>
-      <c r="H3" s="6">
+      <c r="H3" s="8">
         <v>0.134083336591721</v>
       </c>
     </row>
@@ -1058,17 +1133,17 @@
       <c r="B4">
         <v>0.153333333134651</v>
       </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="10">
+      <c r="D4" s="9"/>
+      <c r="E4" s="16">
         <v>3</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="2">
         <v>0.14529166817665101</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G4" s="3">
         <v>0.16250000000000001</v>
       </c>
-      <c r="H4" s="4">
+      <c r="H4" s="10">
         <v>0.13725000023841899</v>
       </c>
     </row>
@@ -1079,17 +1154,17 @@
       <c r="B5">
         <v>0.134083336591721</v>
       </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="10">
+      <c r="D5" s="9"/>
+      <c r="E5" s="16">
         <v>5</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="2">
         <v>0.14029166400432599</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G5" s="3">
         <v>0.178791663050652</v>
       </c>
-      <c r="H5" s="4">
+      <c r="H5" s="10">
         <v>0.141875000298023</v>
       </c>
     </row>
@@ -1100,17 +1175,17 @@
       <c r="B6">
         <v>6.9791668094694601E-2</v>
       </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="10">
+      <c r="D6" s="11"/>
+      <c r="E6" s="17">
         <v>10</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="12">
         <v>6.9791668094694601E-2</v>
       </c>
-      <c r="G6" s="4">
+      <c r="G6" s="13">
         <v>0.18175000250339499</v>
       </c>
-      <c r="H6" s="4">
+      <c r="H6" s="14">
         <v>0.13879166543483701</v>
       </c>
     </row>

</xml_diff>